<commit_message>
commencement de la version 2 avec les comptes
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -443,6 +443,8 @@
     <col width="40" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -469,17 +471,17 @@
     <row r="4">
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>RÉSULTAT date-mois-jours</t>
+          <t>BUDGET année</t>
         </is>
       </c>
       <c r="I4" s="4" t="inlineStr">
         <is>
-          <t>arvida</t>
+          <t>SAINT-DOMINIQUE</t>
         </is>
       </c>
       <c r="J4" s="4" t="inlineStr">
         <is>
-          <t>kenogami</t>
+          <t>SAINTE-FAMILLE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
depenses finalisé à 99$ manque que les totaux a formater
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c402c09f2413666/Bureau/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_2BB1C4B4DDEAD7BAB6C9649257BC98B57D71E269" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F89951C7-0795-49F3-8607-0D900A3135B6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_2BB1C4B4DD9AD5656B2C57B2516318765131E683" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="2400" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>REGROUPEMENT DES PAROISSES</t>
   </si>
@@ -105,13 +105,22 @@
   </si>
   <si>
     <t>revenus autres</t>
+  </si>
+  <si>
+    <t>TOTAL REVENUS DES AUTRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAND  TOTAL REVENUS </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\$"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +146,11 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -175,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,9 +204,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:L25"/>
+  <dimension ref="D2:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,10 +567,10 @@
       <c r="G7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="8">
         <v>10805.56</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="8">
         <v>10805.56</v>
       </c>
     </row>
@@ -568,10 +581,10 @@
       <c r="G8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="8">
         <v>250</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="8">
         <v>250</v>
       </c>
     </row>
@@ -582,10 +595,10 @@
       <c r="G9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="8">
         <v>417.65</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="8">
         <v>417.65</v>
       </c>
     </row>
@@ -596,10 +609,10 @@
       <c r="G10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="8">
         <v>4744.3999999999996</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="8">
         <v>4744.3999999999996</v>
       </c>
     </row>
@@ -610,10 +623,10 @@
       <c r="G11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="7">
-        <v>0</v>
-      </c>
-      <c r="J11" s="7">
+      <c r="I11" s="8">
+        <v>0</v>
+      </c>
+      <c r="J11" s="8">
         <v>0</v>
       </c>
     </row>
@@ -624,10 +637,10 @@
       <c r="G12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="7">
-        <v>0</v>
-      </c>
-      <c r="J12" s="7">
+      <c r="I12" s="8">
+        <v>0</v>
+      </c>
+      <c r="J12" s="8">
         <v>0</v>
       </c>
     </row>
@@ -638,10 +651,10 @@
       <c r="G13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="7">
-        <v>0</v>
-      </c>
-      <c r="J13" s="7">
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
+      <c r="J13" s="8">
         <v>0</v>
       </c>
     </row>
@@ -652,10 +665,10 @@
       <c r="G14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="7">
-        <v>0</v>
-      </c>
-      <c r="J14" s="7">
+      <c r="I14" s="8">
+        <v>0</v>
+      </c>
+      <c r="J14" s="8">
         <v>0</v>
       </c>
     </row>
@@ -666,10 +679,10 @@
       <c r="G15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="8">
         <v>105</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="8">
         <v>105</v>
       </c>
     </row>
@@ -680,10 +693,10 @@
       <c r="G16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="8">
         <v>727.25</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="8">
         <v>727.25</v>
       </c>
     </row>
@@ -694,10 +707,10 @@
       <c r="G17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="8">
         <v>119.45</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="8">
         <v>119.45</v>
       </c>
     </row>
@@ -705,12 +718,12 @@
       <c r="F18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I18">
-        <f>SUM(I7:I17)</f>
-        <v>17169.310000000001</v>
+      <c r="I18" t="e">
+        <f ca="1">SOMME(I7:I17)</f>
+        <v>#NAME?</v>
       </c>
       <c r="J18" t="e">
-        <f ca="1">I8SOMME(J7:J17)</f>
+        <f ca="1">SOMME(J7:J17)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -720,73 +733,99 @@
       </c>
     </row>
     <row r="21" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F21" s="8">
+      <c r="F21" s="6">
         <v>50100</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="8">
         <v>15600</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="8">
         <v>15600</v>
       </c>
     </row>
     <row r="22" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F22" s="8">
+      <c r="F22" s="6">
         <v>50200</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
+      <c r="I22" s="8">
+        <v>0</v>
+      </c>
+      <c r="J22" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>50300</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
+      <c r="I23" s="8">
+        <v>0</v>
+      </c>
+      <c r="J23" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="8">
+      <c r="F24" s="6">
         <v>50400</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
+      <c r="I24" s="8">
+        <v>0</v>
+      </c>
+      <c r="J24" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F25" s="8">
+      <c r="F25" s="6">
         <v>59000</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="8">
         <v>1400.01</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="8">
         <v>1400.01</v>
+      </c>
+    </row>
+    <row r="26" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" t="e">
+        <f ca="1">SOMME(I21:I25)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="J26" t="e">
+        <f ca="1">SOMME(J21:J25)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="28" spans="6:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="F28" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" t="e">
+        <f ca="1">SOMME(I21:I25)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="J28" t="e">
+        <f ca="1">SOMME(J21:J25)</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regroupement terminer et totaux des sections aussi
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -8,32 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c402c09f2413666/Bureau/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_2BB1C4B4DD9AD5656B2C57B2516318765131E683" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_18C926B3DD3AD324E7D815D1535ED87656CDFD07" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>REGROUPEMENT DES PAROISSES</t>
   </si>
@@ -111,6 +98,105 @@
   </si>
   <si>
     <t xml:space="preserve">GRAND  TOTAL REVENUS </t>
+  </si>
+  <si>
+    <t>DÉPENSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  PASTORALE</t>
+  </si>
+  <si>
+    <t>MINISTÈRE</t>
+  </si>
+  <si>
+    <t>FRAIS DE VOYAGE</t>
+  </si>
+  <si>
+    <t>FEUILLET PAROISSIAL</t>
+  </si>
+  <si>
+    <t>cultes</t>
+  </si>
+  <si>
+    <t>UNITÉ DES DEUX-RIVES</t>
+  </si>
+  <si>
+    <t>ANIMATION LITURGIQUE</t>
+  </si>
+  <si>
+    <t>ANIMATION PASTORALE</t>
+  </si>
+  <si>
+    <t>PART ÉGLISE</t>
+  </si>
+  <si>
+    <t>OBJETS DE REVENTE</t>
+  </si>
+  <si>
+    <t>CIMETIÈRE</t>
+  </si>
+  <si>
+    <t>Quêtes commandéée</t>
+  </si>
+  <si>
+    <t>TRIBUT DIOCÉSAIN</t>
+  </si>
+  <si>
+    <t>TOTAL DÉPENSES DE PASTORALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DE BUREAU</t>
+  </si>
+  <si>
+    <t>DÉPENSES DE BUREAU</t>
+  </si>
+  <si>
+    <t>HONORAIRES ET CONTRATS</t>
+  </si>
+  <si>
+    <t>FORMATION</t>
+  </si>
+  <si>
+    <t>ADMINISTRATION/TPS et TVQ</t>
+  </si>
+  <si>
+    <t>CIVILITÉES</t>
+  </si>
+  <si>
+    <t>AUTRE DÉPENSES DE BUREAU</t>
+  </si>
+  <si>
+    <t>SALAIRE ET C.E. EMPLOYEUR</t>
+  </si>
+  <si>
+    <t>TOTAL DÉPENSE DE BUREAU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DE BÂTISSE</t>
+  </si>
+  <si>
+    <t>CHAUFFAGE</t>
+  </si>
+  <si>
+    <t>ÉLECTRICITÉ</t>
+  </si>
+  <si>
+    <t>ENTRETIEN INTÉRIEUR</t>
+  </si>
+  <si>
+    <t>ENTRETIEN EXTÉRIEUR</t>
+  </si>
+  <si>
+    <t>RÉPARATIONS MAJEURES</t>
+  </si>
+  <si>
+    <t>ASSURANCE</t>
+  </si>
+  <si>
+    <t>AUTRE DÉPENSES SUR BÂTISSES</t>
+  </si>
+  <si>
+    <t>TOTAL DÉPENSE DE BÂTISSE</t>
   </si>
 </sst>
 </file>
@@ -189,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -205,6 +291,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -508,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:L28"/>
+  <dimension ref="D2:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,13 +805,11 @@
       <c r="F18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I18" t="e">
-        <f ca="1">SOMME(I7:I17)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J18" t="e">
-        <f ca="1">SOMME(J7:J17)</f>
-        <v>#NAME?</v>
+      <c r="I18" s="9">
+        <v>17169.310000000001</v>
+      </c>
+      <c r="J18" s="9">
+        <v>17169.310000000001</v>
       </c>
     </row>
     <row r="20" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -806,26 +891,464 @@
       <c r="F26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I26" t="e">
-        <f ca="1">SOMME(I21:I25)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J26" t="e">
-        <f ca="1">SOMME(J21:J25)</f>
-        <v>#NAME?</v>
+      <c r="I26">
+        <v>17000.009999999998</v>
+      </c>
+      <c r="J26">
+        <v>17000.009999999998</v>
       </c>
     </row>
     <row r="28" spans="6:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I28" t="e">
-        <f ca="1">SOMME(I21:I25)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J28" t="e">
-        <f ca="1">SOMME(J21:J25)</f>
-        <v>#NAME?</v>
+      <c r="I28">
+        <v>34169.32</v>
+      </c>
+      <c r="J28">
+        <v>34169.32</v>
+      </c>
+    </row>
+    <row r="31" spans="6:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F31" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F32" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F33" s="6">
+        <v>60200</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" s="8">
+        <v>920</v>
+      </c>
+      <c r="J33" s="8">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="34" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F34" s="6">
+        <v>60300</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34" s="8">
+        <v>40</v>
+      </c>
+      <c r="J34" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F35" s="6">
+        <v>60400</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" s="8">
+        <v>0</v>
+      </c>
+      <c r="J35" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F36" s="6">
+        <v>60500</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="8">
+        <v>0</v>
+      </c>
+      <c r="J36" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F37" s="6">
+        <v>60600</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="8">
+        <v>0</v>
+      </c>
+      <c r="J37" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F38" s="6">
+        <v>60700</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I38" s="8">
+        <v>0</v>
+      </c>
+      <c r="J38" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F39" s="6">
+        <v>60800</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I39" s="8">
+        <v>0</v>
+      </c>
+      <c r="J39" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F40" s="6">
+        <v>60900</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I40" s="8">
+        <v>0</v>
+      </c>
+      <c r="J40" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F41" s="6">
+        <v>61000</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I41" s="8">
+        <v>0</v>
+      </c>
+      <c r="J41" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F42" s="6">
+        <v>61100</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I42" s="8">
+        <v>0</v>
+      </c>
+      <c r="J42" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F43" s="6">
+        <v>61200</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I43" s="8">
+        <v>0</v>
+      </c>
+      <c r="J43" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F44" s="6">
+        <v>61300</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I44" s="8">
+        <v>0</v>
+      </c>
+      <c r="J44" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F45" s="6">
+        <v>61400</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I45" s="8">
+        <v>0</v>
+      </c>
+      <c r="J45" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F46" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I46">
+        <v>960</v>
+      </c>
+      <c r="J46">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="48" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F48" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="6">
+        <v>70200</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I49" s="8">
+        <v>898.64</v>
+      </c>
+      <c r="J49" s="8">
+        <v>898.64</v>
+      </c>
+    </row>
+    <row r="50" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F50" s="6">
+        <v>70300</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I50" s="8">
+        <v>545.91</v>
+      </c>
+      <c r="J50" s="8">
+        <v>545.91</v>
+      </c>
+    </row>
+    <row r="51" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F51" s="6">
+        <v>70400</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I51" s="8">
+        <v>105.63</v>
+      </c>
+      <c r="J51" s="8">
+        <v>105.63</v>
+      </c>
+    </row>
+    <row r="52" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F52" s="6">
+        <v>70500</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I52" s="8">
+        <v>328.18</v>
+      </c>
+      <c r="J52" s="8">
+        <v>328.18</v>
+      </c>
+    </row>
+    <row r="53" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F53" s="6">
+        <v>70600</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I53" s="8">
+        <v>346.69000000000011</v>
+      </c>
+      <c r="J53" s="8">
+        <v>346.69000000000011</v>
+      </c>
+    </row>
+    <row r="54" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F54" s="6">
+        <v>79000</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I54" s="8">
+        <v>-123.25</v>
+      </c>
+      <c r="J54" s="8">
+        <v>-123.25</v>
+      </c>
+    </row>
+    <row r="55" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F55" s="6">
+        <v>80100</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I55" s="8">
+        <v>0</v>
+      </c>
+      <c r="J55" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F56" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I56">
+        <v>21041.83</v>
+      </c>
+      <c r="J56">
+        <v>21041.83</v>
+      </c>
+    </row>
+    <row r="58" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F58" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F59" s="6">
+        <v>80200</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I59" s="8">
+        <v>2719.53</v>
+      </c>
+      <c r="J59" s="8">
+        <v>2719.53</v>
+      </c>
+    </row>
+    <row r="60" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F60" s="6">
+        <v>80300</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I60" s="8">
+        <v>978.28</v>
+      </c>
+      <c r="J60" s="8">
+        <v>978.28</v>
+      </c>
+    </row>
+    <row r="61" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F61" s="6">
+        <v>80400</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I61" s="8">
+        <v>108.2</v>
+      </c>
+      <c r="J61" s="8">
+        <v>108.2</v>
+      </c>
+    </row>
+    <row r="62" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F62" s="6">
+        <v>80500</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I62" s="8">
+        <v>3026.54</v>
+      </c>
+      <c r="J62" s="8">
+        <v>3026.54</v>
+      </c>
+    </row>
+    <row r="63" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F63" s="6">
+        <v>80600</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I63" s="8">
+        <v>56.19</v>
+      </c>
+      <c r="J63" s="8">
+        <v>56.19</v>
+      </c>
+    </row>
+    <row r="64" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F64" s="6">
+        <v>80700</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I64" s="8">
+        <v>17897.96</v>
+      </c>
+      <c r="J64" s="8">
+        <v>17897.96</v>
+      </c>
+    </row>
+    <row r="65" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F65" s="6">
+        <v>89000</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I65" s="8">
+        <v>7547.85</v>
+      </c>
+      <c r="J65" s="8">
+        <v>7547.85</v>
+      </c>
+    </row>
+    <row r="66" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F66" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="6:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="F68" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I68">
+        <v>22001.83</v>
+      </c>
+      <c r="J68">
+        <v>22001.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>